<commit_message>
Upload excel file, user test ranking changes
</commit_message>
<xml_diff>
--- a/public/uploads/quiz_question_format.xlsx
+++ b/public/uploads/quiz_question_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sites\quiz\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C11276-2125-4FAC-8D82-2F1098E6B917}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245E51A7-1269-48F6-A333-5AD28CA83B08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,195 +20,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>The Homolographic projection has the correct representation of</t>
+  </si>
+  <si>
+    <t>shape</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>baring</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>The great Victoria Desert is located in</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> West Africa</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Popular in Australia</t>
+  </si>
   <si>
     <t>category_id</t>
   </si>
   <si>
-    <t>option A</t>
-  </si>
-  <si>
-    <t>option B</t>
-  </si>
-  <si>
-    <t>option C</t>
-  </si>
-  <si>
-    <t>option D</t>
-  </si>
-  <si>
-    <t>correct option</t>
-  </si>
-  <si>
-    <t>The Homolographic projection has the correct representation of</t>
-  </si>
-  <si>
-    <t>shape</t>
-  </si>
-  <si>
-    <t>area</t>
-  </si>
-  <si>
-    <t>baring</t>
-  </si>
-  <si>
-    <t>distance</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>The great Victoria Desert is located in</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> West Africa</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>North America</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>The intersecting lines drawn on maps and globes are</t>
-  </si>
-  <si>
-    <t>latitudes</t>
-  </si>
-  <si>
-    <t>longitudes</t>
-  </si>
-  <si>
-    <t>geographic grids</t>
-  </si>
-  <si>
-    <t>None of the above</t>
-  </si>
-  <si>
-    <t>The light of distant stars is affected by</t>
-  </si>
-  <si>
-    <t>the earth's atmosphere</t>
-  </si>
-  <si>
-    <t>interstellar dust</t>
-  </si>
-  <si>
-    <t>both (a) and (bNone of the above</t>
-  </si>
-  <si>
-    <t>The temperature increases rapidly after</t>
-  </si>
-  <si>
-    <t>ionosphere</t>
-  </si>
-  <si>
-    <t>exosphere</t>
-  </si>
-  <si>
-    <t>stratosphere</t>
-  </si>
-  <si>
-    <t>troposphere</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>The humidity of the air depends upon</t>
-  </si>
-  <si>
-    <t>temperature</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>weather</t>
-  </si>
-  <si>
-    <t>All of the above</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>The largest glaciers are</t>
-  </si>
-  <si>
-    <t>mountain glaciers</t>
-  </si>
-  <si>
-    <t>alpine glaciers</t>
-  </si>
-  <si>
-    <t>continental glaciers</t>
-  </si>
-  <si>
-    <t>piedmont glaciers</t>
-  </si>
-  <si>
-    <t>The ionosphere includes</t>
-  </si>
-  <si>
-    <t>mesosphere</t>
-  </si>
-  <si>
-    <t>thermosphere</t>
-  </si>
-  <si>
-    <t>thermosphere and exosphere</t>
-  </si>
-  <si>
-    <t>thermosphere, exosphere and mesosphere</t>
-  </si>
-  <si>
-    <t>The group of minerals chemically containing hydrocarbons is</t>
-  </si>
-  <si>
-    <t>silicate group</t>
-  </si>
-  <si>
-    <t>organic group</t>
-  </si>
-  <si>
-    <t>oxide group</t>
-  </si>
-  <si>
-    <t>hydride group</t>
-  </si>
-  <si>
-    <t>The least explosive type of volcano is called</t>
-  </si>
-  <si>
-    <t>Basalt plateau</t>
-  </si>
-  <si>
-    <t>Cinder cone</t>
-  </si>
-  <si>
-    <t>Shield volcanoes</t>
-  </si>
-  <si>
-    <t>Composite volcanoes</t>
-  </si>
-  <si>
     <t>post_name</t>
   </si>
   <si>
+    <t>option_a</t>
+  </si>
+  <si>
+    <t>option_b</t>
+  </si>
+  <si>
+    <t>option_c</t>
+  </si>
+  <si>
+    <t>option_d</t>
+  </si>
+  <si>
+    <t>correct_option</t>
+  </si>
+  <si>
     <t>explanation</t>
-  </si>
-  <si>
-    <t>Popular in Australia</t>
-  </si>
-  <si>
-    <t>Affected by both</t>
   </si>
 </sst>
 </file>
@@ -216,7 +90,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-4000439]0"/>
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -697,7 +571,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1019,285 +893,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="57.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
     <col min="8" max="8" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>62</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>32</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" t="s">
-        <v>38</v>
-      </c>
+      <c r="A7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
+      <c r="A8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" t="s">
-        <v>17</v>
-      </c>
+      <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" t="s">
-        <v>11</v>
-      </c>
+      <c r="A10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="A11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>